<commit_message>
Historical Work Order View Configuration - HQrHistory
</commit_message>
<xml_diff>
--- a/zero-erp/src/main/resources/plugin/erp/oob/data/erp.wf.view-oa.xlsx
+++ b/zero-erp/src/main/resources/plugin/erp/oob/data/erp.wf.view-oa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/web-app/vertx-zero/vertx-pin/zero-erp/src/main/resources/plugin/erp/oob/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xuanhong\zero-ws\zero-extension\zero-erp\src\main\resources\plugin\erp\oob\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F306065E-18D6-144E-85DA-C9F84145ECAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C0BD7C-4BD8-4975-ACA2-3C54E9BA5980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="38400" windowHeight="22420" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12624" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-MENU" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="142">
   <si>
     <t>key</t>
   </si>
@@ -503,6 +502,10 @@
   </si>
   <si>
     <t>io.vertx.mod.workflow.plugin.query.HQrStandard</t>
+  </si>
+  <si>
+    <t>io.vertx.mod.workflow.plugin.query.HQrHistory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -513,13 +516,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -527,14 +530,14 @@
     <font>
       <sz val="16"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -542,7 +545,7 @@
     <font>
       <sz val="16"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -550,7 +553,7 @@
     <font>
       <sz val="16"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -558,7 +561,7 @@
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -734,7 +737,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -750,7 +753,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1048,30 +1051,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CE16B6-AAB7-164E-9110-1CA8A0C9AC3E}">
   <dimension ref="A2:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F27" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="J46" workbookViewId="0">
+      <selection activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="28.5" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="28.453125" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.36328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="59.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="58" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="28.5" style="3"/>
+    <col min="15" max="16384" width="28.453125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1093,7 +1096,7 @@
       <c r="M2" s="21"/>
       <c r="N2" s="21"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>67</v>
       </c>
@@ -1217,7 +1220,7 @@
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>68</v>
       </c>
@@ -1253,7 +1256,7 @@
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>69</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>70</v>
       </c>
@@ -1329,7 +1332,7 @@
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
@@ -1365,7 +1368,7 @@
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>72</v>
       </c>
@@ -1401,7 +1404,7 @@
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>73</v>
       </c>
@@ -1435,13 +1438,13 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
       <c r="M11" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N11" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>74</v>
       </c>
@@ -1477,7 +1480,7 @@
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>75</v>
       </c>
@@ -1513,7 +1516,7 @@
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>76</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>77</v>
       </c>
@@ -1589,7 +1592,7 @@
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>78</v>
       </c>
@@ -1625,7 +1628,7 @@
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>79</v>
       </c>
@@ -1661,7 +1664,7 @@
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>80</v>
       </c>
@@ -1695,13 +1698,13 @@
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
       <c r="M18" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N18" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>81</v>
       </c>
@@ -1737,7 +1740,7 @@
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -1773,7 +1776,7 @@
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>84</v>
       </c>
@@ -1849,7 +1852,7 @@
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>85</v>
       </c>
@@ -1885,7 +1888,7 @@
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>86</v>
       </c>
@@ -1921,7 +1924,7 @@
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>87</v>
       </c>
@@ -1955,13 +1958,13 @@
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
       <c r="M25" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N25" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>88</v>
       </c>
@@ -1997,7 +2000,7 @@
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>89</v>
       </c>
@@ -2033,7 +2036,7 @@
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>90</v>
       </c>
@@ -2073,7 +2076,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>91</v>
       </c>
@@ -2109,7 +2112,7 @@
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>92</v>
       </c>
@@ -2145,7 +2148,7 @@
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>93</v>
       </c>
@@ -2181,7 +2184,7 @@
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>94</v>
       </c>
@@ -2215,13 +2218,13 @@
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
       <c r="M32" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N32" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>95</v>
       </c>
@@ -2257,7 +2260,7 @@
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>96</v>
       </c>
@@ -2293,7 +2296,7 @@
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>97</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>98</v>
       </c>
@@ -2369,7 +2372,7 @@
       <c r="M36" s="19"/>
       <c r="N36" s="19"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>99</v>
       </c>
@@ -2405,7 +2408,7 @@
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>100</v>
       </c>
@@ -2441,7 +2444,7 @@
       <c r="M38" s="19"/>
       <c r="N38" s="19"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>101</v>
       </c>
@@ -2475,13 +2478,13 @@
       <c r="K39" s="18"/>
       <c r="L39" s="18"/>
       <c r="M39" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N39" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>102</v>
       </c>
@@ -2517,7 +2520,7 @@
       <c r="M40" s="19"/>
       <c r="N40" s="19"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>103</v>
       </c>
@@ -2553,7 +2556,7 @@
       <c r="M41" s="19"/>
       <c r="N41" s="19"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>104</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>105</v>
       </c>
@@ -2629,7 +2632,7 @@
       <c r="M43" s="19"/>
       <c r="N43" s="19"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>106</v>
       </c>
@@ -2665,7 +2668,7 @@
       <c r="M44" s="19"/>
       <c r="N44" s="19"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>107</v>
       </c>
@@ -2701,7 +2704,7 @@
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>108</v>
       </c>
@@ -2735,13 +2738,13 @@
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
       <c r="M46" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N46" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>109</v>
       </c>
@@ -2777,7 +2780,7 @@
       <c r="M47" s="19"/>
       <c r="N47" s="19"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>110</v>
       </c>
@@ -2813,7 +2816,7 @@
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>111</v>
       </c>
@@ -2853,7 +2856,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>112</v>
       </c>
@@ -2889,7 +2892,7 @@
       <c r="M50" s="19"/>
       <c r="N50" s="19"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
         <v>113</v>
       </c>
@@ -2925,7 +2928,7 @@
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>114</v>
       </c>
@@ -2961,7 +2964,7 @@
       <c r="M52" s="19"/>
       <c r="N52" s="19"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>115</v>
       </c>
@@ -2995,13 +2998,13 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
       <c r="M53" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N53" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
         <v>116</v>
       </c>
@@ -3037,7 +3040,7 @@
       <c r="M54" s="19"/>
       <c r="N54" s="19"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
         <v>117</v>
       </c>
@@ -3073,7 +3076,7 @@
       <c r="M55" s="19"/>
       <c r="N55" s="19"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
         <v>118</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
         <v>119</v>
       </c>
@@ -3149,7 +3152,7 @@
       <c r="M57" s="19"/>
       <c r="N57" s="19"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
         <v>120</v>
       </c>
@@ -3185,7 +3188,7 @@
       <c r="M58" s="19"/>
       <c r="N58" s="19"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
         <v>121</v>
       </c>
@@ -3221,7 +3224,7 @@
       <c r="M59" s="19"/>
       <c r="N59" s="19"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
         <v>122</v>
       </c>
@@ -3255,7 +3258,7 @@
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
       <c r="M60" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N60" s="18" t="s">
         <v>139</v>

</xml_diff>